<commit_message>
Files to test the functionality
</commit_message>
<xml_diff>
--- a/massmailer/excel_files/KRA.xlsx
+++ b/massmailer/excel_files/KRA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>AssociateID</t>
   </si>
@@ -31,13 +31,103 @@
     <t>Associate Email</t>
   </si>
   <si>
-    <t>N0628</t>
+    <t>N1070</t>
   </si>
   <si>
     <t>Sreekanth Pogula</t>
   </si>
   <si>
     <t>sreekanth.pogula@senecaglobal.com</t>
+  </si>
+  <si>
+    <t>N1071</t>
+  </si>
+  <si>
+    <t>Bhargavi Gottumukkala</t>
+  </si>
+  <si>
+    <t>bhargavi.gottumukkala@senecaglobal.com</t>
+  </si>
+  <si>
+    <t>N1072</t>
+  </si>
+  <si>
+    <t>Harnath Immani</t>
+  </si>
+  <si>
+    <t>harnath.immani@senecaglobal.com</t>
+  </si>
+  <si>
+    <t>N1073</t>
+  </si>
+  <si>
+    <t>Jawahar Prudhivi</t>
+  </si>
+  <si>
+    <t>jawahar.prudhivi@senecaglobal.com</t>
+  </si>
+  <si>
+    <t>N1074</t>
+  </si>
+  <si>
+    <t>Manisha Siram</t>
+  </si>
+  <si>
+    <t>manisha.siram@senecaglobal.com</t>
+  </si>
+  <si>
+    <t>N1079</t>
+  </si>
+  <si>
+    <t>Nandini Yerrapothu</t>
+  </si>
+  <si>
+    <t>nandini.yerrapothu@senecaglobal.com</t>
+  </si>
+  <si>
+    <t>N1056</t>
+  </si>
+  <si>
+    <t>Prakash Chandra</t>
+  </si>
+  <si>
+    <t>prakash.chandra@senecaglobal.com</t>
+  </si>
+  <si>
+    <t>N1000</t>
+  </si>
+  <si>
+    <t>Ramesh Gidde</t>
+  </si>
+  <si>
+    <t>ramesh.gidde@senecaglobal.com</t>
+  </si>
+  <si>
+    <t>N1234</t>
+  </si>
+  <si>
+    <t>Sabiha Sultana</t>
+  </si>
+  <si>
+    <t>sabiha.sultana@senecaglobal.com</t>
+  </si>
+  <si>
+    <t>N5363</t>
+  </si>
+  <si>
+    <t>Shravani Deshpande</t>
+  </si>
+  <si>
+    <t>shravani.deshpande@senecaglobal.com</t>
+  </si>
+  <si>
+    <t>N3131</t>
+  </si>
+  <si>
+    <t>Yagnabhargavi Penumacha</t>
+  </si>
+  <si>
+    <t>yagnabhargavi.penumacha@senecaglobal.com</t>
   </si>
 </sst>
 </file>
@@ -483,74 +573,174 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final Full fledged product AI
</commit_message>
<xml_diff>
--- a/massmailer/excel_files/KRA.xlsx
+++ b/massmailer/excel_files/KRA.xlsx
@@ -70,10 +70,10 @@
     <t>N1074</t>
   </si>
   <si>
-    <t>Manisha Siram</t>
-  </si>
-  <si>
-    <t>manisha.siram@senecaglobal.com</t>
+    <t>Anusha Kodi</t>
+  </si>
+  <si>
+    <t>anusha.kodi@senecaglobal.com</t>
   </si>
   <si>
     <t>N1079</t>

</xml_diff>

<commit_message>
Added the update code files
</commit_message>
<xml_diff>
--- a/massmailer/excel_files/KRA.xlsx
+++ b/massmailer/excel_files/KRA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="9">
   <si>
     <t>AssociateID</t>
   </si>
@@ -40,94 +40,7 @@
     <t>sreekanth.pogula@senecaglobal.com</t>
   </si>
   <si>
-    <t>N1071</t>
-  </si>
-  <si>
-    <t>Bhargavi Gottumukkala</t>
-  </si>
-  <si>
-    <t>bhargavi.gottumukkala@senecaglobal.com</t>
-  </si>
-  <si>
-    <t>N1072</t>
-  </si>
-  <si>
-    <t>Harnath Immani</t>
-  </si>
-  <si>
-    <t>harnath.immani@senecaglobal.com</t>
-  </si>
-  <si>
-    <t>N1073</t>
-  </si>
-  <si>
-    <t>Jawahar Prudhivi</t>
-  </si>
-  <si>
-    <t>jawahar.prudhivi@senecaglobal.com</t>
-  </si>
-  <si>
-    <t>N1074</t>
-  </si>
-  <si>
-    <t>Anusha Kodi</t>
-  </si>
-  <si>
-    <t>anusha.kodi@senecaglobal.com</t>
-  </si>
-  <si>
-    <t>N1079</t>
-  </si>
-  <si>
-    <t>Nandini Yerrapothu</t>
-  </si>
-  <si>
-    <t>nandini.yerrapothu@senecaglobal.com</t>
-  </si>
-  <si>
-    <t>N1056</t>
-  </si>
-  <si>
-    <t>Prakash Chandra</t>
-  </si>
-  <si>
-    <t>prakash.chandra@senecaglobal.com</t>
-  </si>
-  <si>
-    <t>N1000</t>
-  </si>
-  <si>
-    <t>Ramesh Gidde</t>
-  </si>
-  <si>
-    <t>ramesh.gidde@senecaglobal.com</t>
-  </si>
-  <si>
-    <t>N1234</t>
-  </si>
-  <si>
-    <t>Sabiha Sultana</t>
-  </si>
-  <si>
-    <t>sabiha.sultana@senecaglobal.com</t>
-  </si>
-  <si>
-    <t>N5363</t>
-  </si>
-  <si>
-    <t>Shravani Deshpande</t>
-  </si>
-  <si>
-    <t>shravani.deshpande@senecaglobal.com</t>
-  </si>
-  <si>
-    <t>N3131</t>
-  </si>
-  <si>
-    <t>Yagnabhargavi Penumacha</t>
-  </si>
-  <si>
-    <t>yagnabhargavi.penumacha@senecaglobal.com</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -206,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -218,6 +131,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -531,11 +447,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="26.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="36.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="36.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="39.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="26.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="36.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="36.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="39.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -573,173 +489,173 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>16</v>
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>19</v>
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>22</v>
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>25</v>
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>28</v>
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>31</v>
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>34</v>
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>37</v>
+      <c r="A12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>